<commit_message>
kasur udah siap tapi bug di kaki
</commit_message>
<xml_diff>
--- a/Template KOORDINAT.xlsx
+++ b/Template KOORDINAT.xlsx
@@ -4775,7 +4775,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>X-Desain</t>
   </si>
@@ -4943,10 +4943,13 @@
     <t>ktk_kunci_chest</t>
   </si>
   <si>
+    <t>ktk_bwh_chest2</t>
+  </si>
+  <si>
     <t>ktk_atas_chest2</t>
   </si>
   <si>
-    <t>w_ktk_kunci_chest2</t>
+    <t>ktk_kunci_chest2</t>
   </si>
   <si>
     <t>ktk_jendela</t>
@@ -5557,8 +5560,8 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="poltek" id="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}"/>
-  <person displayName="Neny" id="{A7980FCD-D5B1-027F-FF83-6AE3503CE8DD}"/>
+  <person displayName="poltek" id="{173D1780-D085-D07A-C966-4EEA65435AB2}"/>
+  <person displayName="Neny" id="{32B810E5-130F-77B6-7376-BAC8934697FC}"/>
 </personList>
 </file>
 
@@ -6056,516 +6059,516 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F11" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002500E1-00B8-415B-B628-00BC00C1008B}" done="0">
+  <threadedComment ref="F11" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002500E1-00B8-415B-B628-00BC00C1008B}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F101" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E800CE-007E-426B-B7E5-007C0091000C}" done="0">
+  <threadedComment ref="F101" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E800CE-007E-426B-B7E5-007C0091000C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F102" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E000F6-00AF-4CED-A227-008A00F2001C}" done="0">
+  <threadedComment ref="F102" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E000F6-00AF-4CED-A227-008A00F2001C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F103" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{003D0069-00A4-4EB2-9FF8-00C900CF008C}" done="0">
+  <threadedComment ref="F103" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{003D0069-00A4-4EB2-9FF8-00C900CF008C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F104" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E900E6-0010-43DD-BD1C-002F00250065}" done="0">
+  <threadedComment ref="F104" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E900E6-0010-43DD-BD1C-002F00250065}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F105" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00FE00F5-001D-42E1-AB80-004F006300A1}" done="0">
+  <threadedComment ref="F105" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00FE00F5-001D-42E1-AB80-004F006300A1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F12" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BB00DD-0073-4E2E-8E5F-007C007F0010}" done="0">
+  <threadedComment ref="F12" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BB00DD-0073-4E2E-8E5F-007C007F0010}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F13" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B00031-00C9-4E4A-A3B5-006000A60042}" done="0">
+  <threadedComment ref="F13" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B00031-00C9-4E4A-A3B5-006000A60042}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F14" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{001200B5-0057-4871-9B75-0071006000EE}" done="0">
+  <threadedComment ref="F14" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{001200B5-0057-4871-9B75-0071006000EE}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F15" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0032009A-0014-4A22-A6AB-001F000500BA}" done="0">
+  <threadedComment ref="F15" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0032009A-0014-4A22-A6AB-001F000500BA}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F16" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00CC007D-000D-4589-9961-003000160093}" done="0">
+  <threadedComment ref="F16" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00CC007D-000D-4589-9961-003000160093}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F17" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009400AE-00F2-4CA6-B8A9-00C000DD00B4}" done="0">
+  <threadedComment ref="F17" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009400AE-00F2-4CA6-B8A9-00C000DD00B4}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F18" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{003100D6-0016-4C77-B58E-0060001F0052}" done="0">
+  <threadedComment ref="F18" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{003100D6-0016-4C77-B58E-0060001F0052}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F19" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009D0070-0067-450A-847F-00CD00F5001B}" done="0">
+  <threadedComment ref="F19" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009D0070-0067-450A-847F-00CD00F5001B}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F20" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{006100D3-00DC-44AD-B91D-005F00A0007E}" done="0">
+  <threadedComment ref="F20" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{006100D3-00DC-44AD-B91D-005F00A0007E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F21" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D800F4-000E-4F86-A2C7-0060009400B9}" done="0">
+  <threadedComment ref="F21" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D800F4-000E-4F86-A2C7-0060009400B9}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F22" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{008500D6-0072-416A-8A43-009C0054002E}" done="0">
+  <threadedComment ref="F22" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{008500D6-0072-416A-8A43-009C0054002E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F23" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0089000F-0033-470B-91DC-00C300A40067}" done="0">
+  <threadedComment ref="F23" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0089000F-0033-470B-91DC-00C300A40067}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F24" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{000400E2-0064-464B-8D0F-0091006E00D3}" done="0">
+  <threadedComment ref="F24" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{000400E2-0064-464B-8D0F-0091006E00D3}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F25" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{007E0057-0058-4C50-ABEF-0064004200F8}" done="0">
+  <threadedComment ref="F25" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{007E0057-0058-4C50-ABEF-0064004200F8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F26" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00CC009C-00FA-4C65-A1BB-002300F300AC}" done="0">
+  <threadedComment ref="F26" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00CC009C-00FA-4C65-A1BB-002300F300AC}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F27" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00650033-004D-4692-A5AE-003E005F009E}" done="0">
+  <threadedComment ref="F27" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00650033-004D-4692-A5AE-003E005F009E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F28" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0021000B-00C8-4428-929E-00E600C400BB}" done="0">
+  <threadedComment ref="F28" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0021000B-00C8-4428-929E-00E600C400BB}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F29" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{007300D9-00F6-41C7-A088-009F006F000A}" done="0">
+  <threadedComment ref="F29" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{007300D9-00F6-41C7-A088-009F006F000A}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F30" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0094001B-0027-40F6-BD3E-008A00FC00E9}" done="0">
+  <threadedComment ref="F30" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0094001B-0027-40F6-BD3E-008A00FC00E9}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="E4" personId="{A7980FCD-D5B1-027F-FF83-6AE3503CE8DD}" id="{0061007E-0071-4BA6-9081-003E00590086}" done="0">
+  <threadedComment ref="E4" personId="{32B810E5-130F-77B6-7376-BAC8934697FC}" id="{0061007E-0071-4BA6-9081-003E00590086}" done="0">
     <text xml:space="preserve">isi dengan jumlah piksel yang Anda inginkan untuk tiap milimeter
 </text>
   </threadedComment>
-  <threadedComment ref="F4" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0036007E-0073-472C-A977-006800640035}" done="0">
+  <threadedComment ref="F4" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0036007E-0073-472C-A977-006800640035}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F31" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00FE001C-006A-4714-A502-0091001E00E2}" done="0">
+  <threadedComment ref="F31" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00FE001C-006A-4714-A502-0091001E00E2}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F32" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005400F1-0067-41CE-AAFA-004C00A70066}" done="0">
+  <threadedComment ref="F32" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005400F1-0067-41CE-AAFA-004C00A70066}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F33" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D500C8-00EC-4DA0-B06B-006D002F00C0}" done="0">
+  <threadedComment ref="F33" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D500C8-00EC-4DA0-B06B-006D002F00C0}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F34" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{008500B3-00B1-44A3-BB57-003300300050}" done="0">
+  <threadedComment ref="F34" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{008500B3-00B1-44A3-BB57-003300300050}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F35" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{001500E2-004A-47AE-BD1F-002E004400CF}" done="0">
+  <threadedComment ref="F35" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{001500E2-004A-47AE-BD1F-002E004400CF}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F36" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00560014-0063-4696-B651-0072002E00F1}" done="0">
+  <threadedComment ref="F36" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00560014-0063-4696-B651-0072002E00F1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F37" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BE0009-0085-4D6D-8376-00BD00810093}" done="0">
+  <threadedComment ref="F37" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BE0009-0085-4D6D-8376-00BD00810093}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F38" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BD00DD-00EE-44ED-85E2-003B003C00B5}" done="0">
+  <threadedComment ref="F38" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BD00DD-00EE-44ED-85E2-003B003C00B5}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F39" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{004700F6-0083-4255-BBDD-00A1000B0033}" done="0">
+  <threadedComment ref="F39" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{004700F6-0083-4255-BBDD-00A1000B0033}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F40" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005F009E-001A-40CC-8D4D-0006006800B1}" done="0">
+  <threadedComment ref="F40" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005F009E-001A-40CC-8D4D-0006006800B1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F5" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009500C7-009B-4EE0-AEF2-0092005B009C}" done="0">
+  <threadedComment ref="F5" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009500C7-009B-4EE0-AEF2-0092005B009C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F41" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00240082-00CA-42F1-9880-00ED000200D7}" done="0">
+  <threadedComment ref="F41" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00240082-00CA-42F1-9880-00ED000200D7}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F42" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00570071-00FC-4DA6-A267-0005002300D5}" done="0">
+  <threadedComment ref="F42" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00570071-00FC-4DA6-A267-0005002300D5}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F43" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002E008F-003D-4C92-B908-009F00780064}" done="0">
+  <threadedComment ref="F43" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002E008F-003D-4C92-B908-009F00780064}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F44" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0095000D-00FF-46BD-930B-003800220098}" done="0">
+  <threadedComment ref="F44" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0095000D-00FF-46BD-930B-003800220098}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F45" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00990017-00DC-48C4-82D3-005A00FA0002}" done="0">
+  <threadedComment ref="F45" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00990017-00DC-48C4-82D3-005A00FA0002}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F46" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{007D00FC-0035-4218-96B1-00C3001C00FF}" done="0">
+  <threadedComment ref="F46" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{007D00FC-0035-4218-96B1-00C3001C00FF}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F47" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0070006E-003D-42D8-9D0E-00AD009B00AD}" done="0">
+  <threadedComment ref="F47" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0070006E-003D-42D8-9D0E-00AD009B00AD}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F48" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A700B1-00F5-44A5-9B3A-00E800A6005F}" done="0">
+  <threadedComment ref="F48" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A700B1-00F5-44A5-9B3A-00E800A6005F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F49" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E6004C-00B1-4CE7-A393-009A000B00EF}" done="0">
+  <threadedComment ref="F49" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E6004C-00B1-4CE7-A393-009A000B00EF}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F50" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F20063-0088-4645-82C4-008B001000CE}" done="0">
+  <threadedComment ref="F50" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F20063-0088-4645-82C4-008B001000CE}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F6" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00AD006C-009F-414E-A478-003100110023}" done="0">
+  <threadedComment ref="F6" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00AD006C-009F-414E-A478-003100110023}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F51" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{003A0092-007B-434A-8AE6-00C900550045}" done="0">
+  <threadedComment ref="F51" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{003A0092-007B-434A-8AE6-00C900550045}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F52" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00AC0054-003A-40DE-9700-00ED002D0086}" done="0">
+  <threadedComment ref="F52" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00AC0054-003A-40DE-9700-00ED002D0086}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F53" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{008B0081-00F6-4868-B8C9-009300E0004A}" done="0">
+  <threadedComment ref="F53" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{008B0081-00F6-4868-B8C9-009300E0004A}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F54" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00970002-00F4-4452-BF03-008700B20007}" done="0">
+  <threadedComment ref="F54" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00970002-00F4-4452-BF03-008700B20007}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F55" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00CD00CD-0015-4B47-9901-008200CC0049}" done="0">
+  <threadedComment ref="F55" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00CD00CD-0015-4B47-9901-008200CC0049}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F56" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{003F00CD-0090-45F5-BEFB-003B00BB0042}" done="0">
+  <threadedComment ref="F56" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{003F00CD-0090-45F5-BEFB-003B00BB0042}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F57" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005E0063-004F-4D56-9B30-00CE00600070}" done="0">
+  <threadedComment ref="F57" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005E0063-004F-4D56-9B30-00CE00600070}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F58" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002800EB-00B6-44DF-BEDF-00B300EB0001}" done="0">
+  <threadedComment ref="F58" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002800EB-00B6-44DF-BEDF-00B300EB0001}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F59" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C40096-0089-4182-B76B-00BB006D0082}" done="0">
+  <threadedComment ref="F59" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C40096-0089-4182-B76B-00BB006D0082}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F60" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D20078-00B2-4562-AD8B-00E500D20044}" done="0">
+  <threadedComment ref="F60" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D20078-00B2-4562-AD8B-00E500D20044}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F7" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009600C6-000D-4695-AD6A-00AA00460012}" done="0">
+  <threadedComment ref="F7" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009600C6-000D-4695-AD6A-00AA00460012}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F61" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B200FF-00D5-4A30-9BF7-00EA007A00F8}" done="0">
+  <threadedComment ref="F61" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B200FF-00D5-4A30-9BF7-00EA007A00F8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F62" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00880089-0011-4F44-8646-007B00BB0042}" done="0">
+  <threadedComment ref="F62" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00880089-0011-4F44-8646-007B00BB0042}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F63" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00320017-0039-4020-A31A-00C1006E00E3}" done="0">
+  <threadedComment ref="F63" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00320017-0039-4020-A31A-00C1006E00E3}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F64" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C700AA-0061-48CF-AC77-009B00C1007F}" done="0">
+  <threadedComment ref="F64" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C700AA-0061-48CF-AC77-009B00C1007F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F65" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00AC00BD-009E-4F69-9DA5-009F009400DB}" done="0">
+  <threadedComment ref="F65" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00AC00BD-009E-4F69-9DA5-009F009400DB}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F66" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002D0025-00FA-484A-B277-007100380059}" done="0">
+  <threadedComment ref="F66" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002D0025-00FA-484A-B277-007100380059}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F67" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009E00BC-008A-421F-8CD1-007300E60069}" done="0">
+  <threadedComment ref="F67" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009E00BC-008A-421F-8CD1-007300E60069}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F68" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009400E2-005D-42B8-AEAC-00B20057004C}" done="0">
+  <threadedComment ref="F68" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009400E2-005D-42B8-AEAC-00B20057004C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F69" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00790007-005D-4620-A635-009F008100F1}" done="0">
+  <threadedComment ref="F69" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00790007-005D-4620-A635-009F008100F1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F70" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00DB000D-003C-4972-A55A-001700780095}" done="0">
+  <threadedComment ref="F70" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00DB000D-003C-4972-A55A-001700780095}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F8" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005600E1-0021-450A-A907-006500800023}" done="0">
+  <threadedComment ref="F8" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005600E1-0021-450A-A907-006500800023}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F71" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E200C4-0054-45F0-869E-007100930078}" done="0">
+  <threadedComment ref="F71" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E200C4-0054-45F0-869E-007100930078}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F72" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0056006F-0044-41C1-9237-003D006400D5}" done="0">
+  <threadedComment ref="F72" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0056006F-0044-41C1-9237-003D006400D5}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F73" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E5000A-0043-45C2-AB43-0036008600BC}" done="0">
+  <threadedComment ref="F73" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E5000A-0043-45C2-AB43-0036008600BC}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F74" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00080024-0009-4C90-9AA6-0028006F00C3}" done="0">
+  <threadedComment ref="F74" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00080024-0009-4C90-9AA6-0028006F00C3}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F75" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BF006F-00FD-40E9-BF62-00380095009C}" done="0">
+  <threadedComment ref="F75" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BF006F-00FD-40E9-BF62-00380095009C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F76" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00AC0078-0023-42F0-896E-00B400AC0061}" done="0">
+  <threadedComment ref="F76" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00AC0078-0023-42F0-896E-00B400AC0061}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F77" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B40051-00E4-4EF1-AC80-00DA00AE00A9}" done="0">
+  <threadedComment ref="F77" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B40051-00E4-4EF1-AC80-00DA00AE00A9}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F78" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{001F00EB-00A6-4182-93A2-008200790053}" done="0">
+  <threadedComment ref="F78" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{001F00EB-00A6-4182-93A2-008200790053}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F79" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{008200E4-001B-4421-88B8-00AC0024003B}" done="0">
+  <threadedComment ref="F79" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{008200E4-001B-4421-88B8-00AC0024003B}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F80" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00650063-001C-47BC-8F07-00A4009800C7}" done="0">
+  <threadedComment ref="F80" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00650063-001C-47BC-8F07-00A4009800C7}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F9" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00750071-0023-4422-9A66-00D1003D00CB}" done="0">
+  <threadedComment ref="F9" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00750071-0023-4422-9A66-00D1003D00CB}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F81" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D4003E-0044-4199-9D3C-005900F3009C}" done="0">
+  <threadedComment ref="F81" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D4003E-0044-4199-9D3C-005900F3009C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F82" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00CC000B-00DD-4305-8A0B-00F900EA0068}" done="0">
+  <threadedComment ref="F82" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00CC000B-00DD-4305-8A0B-00F900EA0068}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F83" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00970097-00E6-43CC-8851-008300AF0076}" done="0">
+  <threadedComment ref="F83" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00970097-00E6-43CC-8851-008300AF0076}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F84" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002800BB-00C4-478C-BCF0-005300690023}" done="0">
+  <threadedComment ref="F84" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002800BB-00C4-478C-BCF0-005300690023}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F85" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C10025-0085-4258-BBAF-0047001400B7}" done="0">
+  <threadedComment ref="F85" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C10025-0085-4258-BBAF-0047001400B7}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F86" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00720040-0056-4BFC-BE0B-004A001E006F}" done="0">
+  <threadedComment ref="F86" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00720040-0056-4BFC-BE0B-004A001E006F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F87" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00CD0068-003B-48A9-B257-00A400C30005}" done="0">
+  <threadedComment ref="F87" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00CD0068-003B-48A9-B257-00A400C30005}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F88" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00380059-00CD-4680-903F-001200BC00A4}" done="0">
+  <threadedComment ref="F88" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00380059-00CD-4680-903F-001200BC00A4}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F89" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009500FB-00AD-4626-8417-008800A000E1}" done="0">
+  <threadedComment ref="F89" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009500FB-00AD-4626-8417-008800A000E1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F90" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A1003A-004A-469B-ACBF-000A004500CC}" done="0">
+  <threadedComment ref="F90" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A1003A-004A-469B-ACBF-000A004500CC}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F10" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BE0084-00DB-4A19-AD4C-007200DE000E}" done="0">
+  <threadedComment ref="F10" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BE0084-00DB-4A19-AD4C-007200DE000E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F91" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0046004F-0047-4C64-87E5-00EE00970097}" done="0">
+  <threadedComment ref="F91" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0046004F-0047-4C64-87E5-00EE00970097}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F92" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005100A3-007B-4685-8AC8-008000D800E8}" done="0">
+  <threadedComment ref="F92" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005100A3-007B-4685-8AC8-008000D800E8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F93" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{000600FD-0053-45F8-A391-001900AD00C0}" done="0">
+  <threadedComment ref="F93" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{000600FD-0053-45F8-A391-001900AD00C0}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F94" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E10009-0042-404A-9F0C-00BD006F0031}" done="0">
+  <threadedComment ref="F94" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E10009-0042-404A-9F0C-00BD006F0031}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F95" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00270083-0048-4D3F-9E3F-00F900F700D9}" done="0">
+  <threadedComment ref="F95" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00270083-0048-4D3F-9E3F-00F900F700D9}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F96" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{003F00F7-00D8-427E-9913-003500030020}" done="0">
+  <threadedComment ref="F96" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{003F00F7-00D8-427E-9913-003500030020}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F97" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00960084-0098-4664-BC96-009B00110086}" done="0">
+  <threadedComment ref="F97" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00960084-0098-4664-BC96-009B00110086}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F98" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005C0033-00EA-4983-B8DA-00E100410007}" done="0">
+  <threadedComment ref="F98" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005C0033-00EA-4983-B8DA-00E100410007}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F99" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00950047-001D-4E75-8932-009A002C00E1}" done="0">
+  <threadedComment ref="F99" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00950047-001D-4E75-8932-009A002C00E1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F100" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00DB00DE-0033-4655-BFAD-003B007C0021}" done="0">
+  <threadedComment ref="F100" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00DB00DE-0033-4655-BFAD-003B007C0021}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
@@ -6575,516 +6578,516 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F11" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0019003E-00DD-4011-9D56-005900790044}" done="0">
+  <threadedComment ref="F11" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0019003E-00DD-4011-9D56-005900790044}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F101" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00EB00FE-009E-4709-904D-006B001F001E}" done="0">
+  <threadedComment ref="F101" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00EB00FE-009E-4709-904D-006B001F001E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F102" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D700D5-0053-4DB6-9621-000B009800CB}" done="0">
+  <threadedComment ref="F102" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D700D5-0053-4DB6-9621-000B009800CB}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F103" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{008800FF-0055-4844-ACC2-0076001100CF}" done="0">
+  <threadedComment ref="F103" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{008800FF-0055-4844-ACC2-0076001100CF}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F104" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005400F9-006F-4035-AAB7-0030005800CE}" done="0">
+  <threadedComment ref="F104" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005400F9-006F-4035-AAB7-0030005800CE}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F105" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00CD0083-00F4-4E02-AC89-00F60064008E}" done="0">
+  <threadedComment ref="F105" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00CD0083-00F4-4E02-AC89-00F60064008E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F12" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B1001A-00E3-40E1-9E1D-000D008E008D}" done="0">
+  <threadedComment ref="F12" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B1001A-00E3-40E1-9E1D-000D008E008D}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F13" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B400C0-00D5-40E5-8A1A-00D5009000F4}" done="0">
+  <threadedComment ref="F13" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B400C0-00D5-40E5-8A1A-00D5009000F4}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F14" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00EE00B7-008D-485F-AA06-009400F0002D}" done="0">
+  <threadedComment ref="F14" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00EE00B7-008D-485F-AA06-009400F0002D}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F15" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002E00C1-0009-4AA1-A21E-008600AD00F1}" done="0">
+  <threadedComment ref="F15" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002E00C1-0009-4AA1-A21E-008600AD00F1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F16" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A5002A-008B-4DB1-9909-007100CE0097}" done="0">
+  <threadedComment ref="F16" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A5002A-008B-4DB1-9909-007100CE0097}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F17" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{000200B5-009D-4FD4-8618-00DD00FF001C}" done="0">
+  <threadedComment ref="F17" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{000200B5-009D-4FD4-8618-00DD00FF001C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F18" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C700DB-001C-43D6-B0B8-00650049008E}" done="0">
+  <threadedComment ref="F18" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C700DB-001C-43D6-B0B8-00650049008E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F19" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00020099-007C-4D6A-AB89-00BB006100C9}" done="0">
+  <threadedComment ref="F19" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00020099-007C-4D6A-AB89-00BB006100C9}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F20" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B200A1-00A5-4B96-8E58-007B000A004A}" done="0">
+  <threadedComment ref="F20" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B200A1-00A5-4B96-8E58-007B000A004A}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F21" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00AA007B-0069-441C-B70A-00B3007F00A4}" done="0">
+  <threadedComment ref="F21" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00AA007B-0069-441C-B70A-00B3007F00A4}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F22" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C50050-0073-40FC-9B5F-009800E000B2}" done="0">
+  <threadedComment ref="F22" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C50050-0073-40FC-9B5F-009800E000B2}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F23" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D20041-00C8-4C87-93B6-002F000B00D5}" done="0">
+  <threadedComment ref="F23" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D20041-00C8-4C87-93B6-002F000B00D5}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F24" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0006001B-006F-4061-88D4-00CE00BC00D3}" done="0">
+  <threadedComment ref="F24" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0006001B-006F-4061-88D4-00CE00BC00D3}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F25" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00EA00B5-00FA-4937-A378-007F00CE00EE}" done="0">
+  <threadedComment ref="F25" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00EA00B5-00FA-4937-A378-007F00CE00EE}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F26" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0096009B-00C3-4BC1-BF79-0073004D00DA}" done="0">
+  <threadedComment ref="F26" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0096009B-00C3-4BC1-BF79-0073004D00DA}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F27" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00660028-0017-4593-8105-00D500CA00CF}" done="0">
+  <threadedComment ref="F27" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00660028-0017-4593-8105-00D500CA00CF}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F28" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0054003B-00EA-4C66-B79C-00CF00F600D3}" done="0">
+  <threadedComment ref="F28" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0054003B-00EA-4C66-B79C-00CF00F600D3}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F29" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{008E00DA-0015-49B4-A1FF-005F00BA00B8}" done="0">
+  <threadedComment ref="F29" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{008E00DA-0015-49B4-A1FF-005F00BA00B8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F30" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00DF00B9-00FF-4510-8F78-0064004D0062}" done="0">
+  <threadedComment ref="F30" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00DF00B9-00FF-4510-8F78-0064004D0062}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="E4" personId="{A7980FCD-D5B1-027F-FF83-6AE3503CE8DD}" id="{007900C2-005E-48A6-8CBD-0036008F00C9}" done="0">
+  <threadedComment ref="E4" personId="{32B810E5-130F-77B6-7376-BAC8934697FC}" id="{007900C2-005E-48A6-8CBD-0036008F00C9}" done="0">
     <text xml:space="preserve">isi dengan jumlah piksel yang Anda inginkan untuk tiap milimeter
 </text>
   </threadedComment>
-  <threadedComment ref="F4" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0034000F-00E9-4A7B-BC67-00AE00910055}" done="0">
+  <threadedComment ref="F4" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0034000F-00E9-4A7B-BC67-00AE00910055}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F31" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E600E5-00FE-4E84-9545-0024006F00A3}" done="0">
+  <threadedComment ref="F31" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E600E5-00FE-4E84-9545-0024006F00A3}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F32" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0012003B-00C3-4448-86A4-000A0049004B}" done="0">
+  <threadedComment ref="F32" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0012003B-00C3-4448-86A4-000A0049004B}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F33" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00240072-0031-4FCF-8345-006E00710052}" done="0">
+  <threadedComment ref="F33" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00240072-0031-4FCF-8345-006E00710052}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F34" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00AD0072-00EF-4B0A-904A-00DF002000C2}" done="0">
+  <threadedComment ref="F34" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00AD0072-00EF-4B0A-904A-00DF002000C2}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F35" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00DF00C8-00EA-4D94-8C52-00050096005E}" done="0">
+  <threadedComment ref="F35" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00DF00C8-00EA-4D94-8C52-00050096005E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F36" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E8008E-0075-4E96-BD3B-003A00D20034}" done="0">
+  <threadedComment ref="F36" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E8008E-0075-4E96-BD3B-003A00D20034}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F37" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F000DA-0053-4C2E-B776-00E100FD00E6}" done="0">
+  <threadedComment ref="F37" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F000DA-0053-4C2E-B776-00E100FD00E6}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F38" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0007002B-00A0-47A9-A420-002E00BA0073}" done="0">
+  <threadedComment ref="F38" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0007002B-00A0-47A9-A420-002E00BA0073}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F39" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{004E00A9-00B1-451A-A379-00E900300036}" done="0">
+  <threadedComment ref="F39" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{004E00A9-00B1-451A-A379-00E900300036}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F40" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00400002-0059-4D59-A276-00CB00E40084}" done="0">
+  <threadedComment ref="F40" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00400002-0059-4D59-A276-00CB00E40084}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F5" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00AA0075-00D0-4936-8B93-00F600E30056}" done="0">
+  <threadedComment ref="F5" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00AA0075-00D0-4936-8B93-00F600E30056}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F41" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{007A003A-0052-4D44-BE5F-002700A3008A}" done="0">
+  <threadedComment ref="F41" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{007A003A-0052-4D44-BE5F-002700A3008A}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F42" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005900EB-00EE-41D5-BBC7-004500230082}" done="0">
+  <threadedComment ref="F42" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005900EB-00EE-41D5-BBC7-004500230082}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F43" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0066006C-0075-4910-9BBE-007300B600D2}" done="0">
+  <threadedComment ref="F43" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0066006C-0075-4910-9BBE-007300B600D2}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F44" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BD0039-0060-4A32-A1FA-00EB00620059}" done="0">
+  <threadedComment ref="F44" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BD0039-0060-4A32-A1FA-00EB00620059}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F45" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{003600C2-002B-4BB3-94AF-00F000610003}" done="0">
+  <threadedComment ref="F45" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{003600C2-002B-4BB3-94AF-00F000610003}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F46" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C8007C-00BE-4CF5-A05E-00D30007004E}" done="0">
+  <threadedComment ref="F46" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C8007C-00BE-4CF5-A05E-00D30007004E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F47" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BE00EB-0060-4465-86B7-00F400EF0075}" done="0">
+  <threadedComment ref="F47" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BE00EB-0060-4465-86B7-00F400EF0075}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F48" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{003A00B1-0087-4036-9277-004D00D600C2}" done="0">
+  <threadedComment ref="F48" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{003A00B1-0087-4036-9277-004D00D600C2}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F49" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{001B00D1-0043-47CD-B36D-008100A200E8}" done="0">
+  <threadedComment ref="F49" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{001B00D1-0043-47CD-B36D-008100A200E8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F50" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D80008-00BB-4263-8E96-003F00A4004A}" done="0">
+  <threadedComment ref="F50" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D80008-00BB-4263-8E96-003F00A4004A}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F6" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{001E00CE-0048-475C-8F03-005D00FC00AB}" done="0">
+  <threadedComment ref="F6" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{001E00CE-0048-475C-8F03-005D00FC00AB}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F51" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{008A008F-00C4-42A2-9BB4-0012001B001F}" done="0">
+  <threadedComment ref="F51" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{008A008F-00C4-42A2-9BB4-0012001B001F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F52" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009F004E-00F7-4254-A488-002600110066}" done="0">
+  <threadedComment ref="F52" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009F004E-00F7-4254-A488-002600110066}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F53" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F400D7-00E7-4B49-837A-00DF008D009C}" done="0">
+  <threadedComment ref="F53" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F400D7-00E7-4B49-837A-00DF008D009C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F54" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009B005D-00D2-427C-969A-0004003400E3}" done="0">
+  <threadedComment ref="F54" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009B005D-00D2-427C-969A-0004003400E3}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F55" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0099001A-0080-4833-A44C-00F1006F00ED}" done="0">
+  <threadedComment ref="F55" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0099001A-0080-4833-A44C-00F1006F00ED}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F56" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D40085-001B-4138-9210-00CC00400091}" done="0">
+  <threadedComment ref="F56" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D40085-001B-4138-9210-00CC00400091}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F57" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002E00E5-00AA-4A4B-885A-00D3006400A8}" done="0">
+  <threadedComment ref="F57" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002E00E5-00AA-4A4B-885A-00D3006400A8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F58" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A900F6-00CA-4FBB-A637-006D00E900DE}" done="0">
+  <threadedComment ref="F58" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A900F6-00CA-4FBB-A637-006D00E900DE}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F59" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F90006-0053-4D67-A51B-003900E70039}" done="0">
+  <threadedComment ref="F59" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F90006-0053-4D67-A51B-003900E70039}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F60" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009600A0-0064-49EE-9A88-00DF00D30094}" done="0">
+  <threadedComment ref="F60" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009600A0-0064-49EE-9A88-00DF00D30094}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F7" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00FB0041-006D-481D-B14B-0088007300C8}" done="0">
+  <threadedComment ref="F7" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00FB0041-006D-481D-B14B-0088007300C8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F61" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B100BB-004B-4978-8955-005500AE0057}" done="0">
+  <threadedComment ref="F61" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B100BB-004B-4978-8955-005500AE0057}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F62" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00DC0093-0025-4048-A61E-001E00F40032}" done="0">
+  <threadedComment ref="F62" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00DC0093-0025-4048-A61E-001E00F40032}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F63" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009E007C-0048-45D6-A57A-00A8007200F8}" done="0">
+  <threadedComment ref="F63" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009E007C-0048-45D6-A57A-00A8007200F8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F64" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C900D3-00F2-4872-AAF9-00B1000400BB}" done="0">
+  <threadedComment ref="F64" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C900D3-00F2-4872-AAF9-00B1000400BB}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F65" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A600C9-0097-4674-BC98-00DB002800A0}" done="0">
+  <threadedComment ref="F65" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A600C9-0097-4674-BC98-00DB002800A0}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F66" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{000500AF-00D3-450D-A721-004000E8008B}" done="0">
+  <threadedComment ref="F66" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{000500AF-00D3-450D-A721-004000E8008B}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F67" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005A00B9-0067-4B9F-8A50-00EB00570045}" done="0">
+  <threadedComment ref="F67" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005A00B9-0067-4B9F-8A50-00EB00570045}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F68" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00FC00A7-0005-495C-9302-0032006A006C}" done="0">
+  <threadedComment ref="F68" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00FC00A7-0005-495C-9302-0032006A006C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F69" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A50048-00DE-4A19-8C0A-00140082002E}" done="0">
+  <threadedComment ref="F69" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A50048-00DE-4A19-8C0A-00140082002E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F70" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A200D8-0028-455C-8EBD-0078008900C6}" done="0">
+  <threadedComment ref="F70" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A200D8-0028-455C-8EBD-0078008900C6}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F8" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00960079-0077-4F2A-82A2-00BD00C3007F}" done="0">
+  <threadedComment ref="F8" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00960079-0077-4F2A-82A2-00BD00C3007F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F71" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00DF003A-001B-4DB1-9E42-007400AC00E1}" done="0">
+  <threadedComment ref="F71" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00DF003A-001B-4DB1-9E42-007400AC00E1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F72" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F3005C-00CA-4F2D-B387-0081004F009E}" done="0">
+  <threadedComment ref="F72" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F3005C-00CA-4F2D-B387-0081004F009E}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F73" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{007C0051-009E-4FFD-B2F5-00C600D50053}" done="0">
+  <threadedComment ref="F73" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{007C0051-009E-4FFD-B2F5-00C600D50053}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F74" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00670022-0015-4186-BA4E-009B000F0061}" done="0">
+  <threadedComment ref="F74" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00670022-0015-4186-BA4E-009B000F0061}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F75" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00500052-00E0-4AB2-9BBE-00A5009600C1}" done="0">
+  <threadedComment ref="F75" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00500052-00E0-4AB2-9BBE-00A5009600C1}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F76" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F0004F-0064-499D-801C-000700D3002F}" done="0">
+  <threadedComment ref="F76" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F0004F-0064-499D-801C-000700D3002F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F77" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{001400B2-00F1-4DB3-9DE7-00A000150039}" done="0">
+  <threadedComment ref="F77" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{001400B2-00F1-4DB3-9DE7-00A000150039}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F78" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{002400EE-00C1-4E63-80AA-009F004E0000}" done="0">
+  <threadedComment ref="F78" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{002400EE-00C1-4E63-80AA-009F004E0000}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F79" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A2005A-00E8-4C73-BE0C-009600930058}" done="0">
+  <threadedComment ref="F79" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A2005A-00E8-4C73-BE0C-009600930058}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F80" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00FE004A-004D-4DC5-9616-00FE006100BC}" done="0">
+  <threadedComment ref="F80" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00FE004A-004D-4DC5-9616-00FE006100BC}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F9" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00DC0029-00E7-42DB-B9C1-003400EA0062}" done="0">
+  <threadedComment ref="F9" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00DC0029-00E7-42DB-B9C1-003400EA0062}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F81" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00E200BC-0050-488A-B834-006200C90035}" done="0">
+  <threadedComment ref="F81" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00E200BC-0050-488A-B834-006200C90035}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F82" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F700FA-0046-463B-90CC-00EC005200E4}" done="0">
+  <threadedComment ref="F82" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F700FA-0046-463B-90CC-00EC005200E4}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F83" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00A8006C-009A-4446-8DF2-005000F800A8}" done="0">
+  <threadedComment ref="F83" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00A8006C-009A-4446-8DF2-005000F800A8}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F84" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00BC003C-00E7-4887-9335-00BE00A00084}" done="0">
+  <threadedComment ref="F84" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00BC003C-00E7-4887-9335-00BE00A00084}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F85" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D3001D-0010-45EF-BB8A-0054009E00B0}" done="0">
+  <threadedComment ref="F85" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D3001D-0010-45EF-BB8A-0054009E00B0}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F86" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00F80095-0024-4050-BFE8-002A000A0063}" done="0">
+  <threadedComment ref="F86" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00F80095-0024-4050-BFE8-002A000A0063}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F87" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0004000B-00D2-4380-8028-006600E5001D}" done="0">
+  <threadedComment ref="F87" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0004000B-00D2-4380-8028-006600E5001D}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F88" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{006100B6-00A0-44B1-954A-006400C90072}" done="0">
+  <threadedComment ref="F88" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{006100B6-00A0-44B1-954A-006400C90072}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F89" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{007E0001-00BA-4A1B-BFEA-009C000B003F}" done="0">
+  <threadedComment ref="F89" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{007E0001-00BA-4A1B-BFEA-009C000B003F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F90" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{006D000D-00B1-4850-80B6-001C002B00C4}" done="0">
+  <threadedComment ref="F90" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{006D000D-00B1-4850-80B6-001C002B00C4}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F10" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00B7001B-00DB-4B45-809D-00D000730097}" done="0">
+  <threadedComment ref="F10" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00B7001B-00DB-4B45-809D-00D000730097}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F91" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{005F00B7-0068-4E20-B708-00B1008000A5}" done="0">
+  <threadedComment ref="F91" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{005F00B7-0068-4E20-B708-00B1008000A5}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F92" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00D2000D-008E-4F0E-889B-008D00540073}" done="0">
+  <threadedComment ref="F92" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00D2000D-008E-4F0E-889B-008D00540073}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F93" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00720077-00F3-41DB-80E4-00E6002900BA}" done="0">
+  <threadedComment ref="F93" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00720077-00F3-41DB-80E4-00E6002900BA}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F94" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00C70063-00A4-4E22-8B1D-008900470066}" done="0">
+  <threadedComment ref="F94" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00C70063-00A4-4E22-8B1D-008900470066}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F95" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00EF00A4-00D5-4A7C-AA4A-001D00140024}" done="0">
+  <threadedComment ref="F95" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00EF00A4-00D5-4A7C-AA4A-001D00140024}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F96" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{007A0009-008B-48C0-98F5-007E00320029}" done="0">
+  <threadedComment ref="F96" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{007A0009-008B-48C0-98F5-007E00320029}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F97" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{00490001-00FB-48E3-A81C-008400EF00B4}" done="0">
+  <threadedComment ref="F97" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{00490001-00FB-48E3-A81C-008400EF00B4}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F98" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{0053002C-0058-412F-A5E0-00F5008A0042}" done="0">
+  <threadedComment ref="F98" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{0053002C-0058-412F-A5E0-00F5008A0042}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F99" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{004800D8-003D-401F-B7E7-0098004A006C}" done="0">
+  <threadedComment ref="F99" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{004800D8-003D-401F-B7E7-0098004A006C}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
   </threadedComment>
-  <threadedComment ref="F100" personId="{48F801F5-A39B-FEA3-88E2-8AE7F7265A9F}" id="{009600AA-0088-47E1-85DE-007F0056006F}" done="0">
+  <threadedComment ref="F100" personId="{173D1780-D085-D07A-C966-4EEA65435AB2}" id="{009600AA-0088-47E1-85DE-007F0056006F}" done="0">
     <text xml:space="preserve">1 = set RGB
 2 = set Koordinat
 </text>
@@ -18353,7 +18356,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{0058001F-007E-4FBA-9451-00B00045008A}">
+          <x14:cfRule type="expression" priority="3" id="{00110013-0094-48A8-AEF1-00C000D900EF}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -18370,7 +18373,7 @@
           <xm:sqref>J4:J105</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{00B000D4-006B-4EF0-ACA0-00A000FE00D2}">
+          <x14:cfRule type="expression" priority="2" id="{00BB00F3-0083-4160-9D96-009A00BF0063}">
             <xm:f>$F4=2</xm:f>
             <x14:dxf>
               <font>
@@ -18387,7 +18390,7 @@
           <xm:sqref>K4:M105</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{008C00A4-0075-4818-95EC-006500DB00F9}">
+          <x14:cfRule type="expression" priority="1" id="{0039005A-0019-4193-A44C-00150041005F}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -18407,25 +18410,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E40049-0005-425A-BB1F-00CB004800C4}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= LEBAR DESAIN" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001F003E-006B-4930-B984-004100E40050}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= LEBAR DESAIN" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>AF4:AR105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0049005D-005E-4F77-8F9F-003F00F9004A}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 768" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F500FE-0099-4792-A744-008600FE0044}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 768" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>768</xm:f>
           </x14:formula1>
           <xm:sqref>B4 D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006100FD-00F0-4368-AEE2-001C00FD005D}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 1024" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007A0074-00EF-461B-8CF7-00FB00980058}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 1024" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>1024</xm:f>
           </x14:formula1>
           <xm:sqref>A4 C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009C0070-00C8-41D8-A014-0024006300CB}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F300FD-002A-4CA3-A0AD-00CF00890030}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>1</xm:f>
           </x14:formula1>
@@ -18434,19 +18437,19 @@
           </x14:formula2>
           <xm:sqref>F4:F105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008A004E-00EC-4340-BD91-00A3003B0010}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Diisi banyaknya titik" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EE005E-0082-43AA-8E49-0044003E000E}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Diisi banyaknya titik" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>AND(F4=2,J4&gt;0)</xm:f>
           </x14:formula1>
           <xm:sqref>J4:J105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004900A5-00EB-4EEC-B227-008E008D00E5}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Isi dengan angka 0 - 255" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D50008-00D9-4C7D-93C3-00DB00E40080}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Isi dengan angka 0 - 255" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>AND($F4=1,K4&gt;=0,K4&lt;256)</xm:f>
           </x14:formula1>
           <xm:sqref>K4:M105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007C00B3-0093-49B1-B239-009600C100E9}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00230007-0002-4EF2-AA6E-008E00030071}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
@@ -21370,13 +21373,13 @@
         <v>7.5</v>
       </c>
       <c r="S25" s="49">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T25" s="43">
         <v>7.5</v>
       </c>
       <c r="U25" s="50">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="V25" s="48">
         <v>10</v>
@@ -21403,7 +21406,7 @@
       </c>
       <c r="AG25" s="54">
         <f t="shared" si="43"/>
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="AH25" s="55">
         <f t="shared" si="43"/>
@@ -21411,7 +21414,7 @@
       </c>
       <c r="AI25" s="52">
         <f t="shared" si="43"/>
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="AJ25" s="53">
         <f t="shared" si="43"/>
@@ -21451,7 +21454,7 @@
       </c>
       <c r="AS25" s="57" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">Point2D_t  ktk_palu [4] = {{248.,30.},{268.,30.},{268.,40.},{248.,40.},{.,.},{.,.},{.,.}};</v>
+        <v xml:space="preserve">Point2D_t  ktk_palu [4] = {{248.,30.},{272.,30.},{272.,40.},{248.,40.},{.,.},{.,.},{.,.}};</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1">
@@ -24269,7 +24272,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I49" s="42" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="J49" s="43"/>
       <c r="K49" s="38"/>
@@ -24375,7 +24378,7 @@
       </c>
       <c r="AS49" s="57" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">Point2D_t  ktk_bwh_chest [] = {{500.,80.},{660.,80.},{660.,120.},{500.,120.},{.,.},{.,.},{.,.}};</v>
+        <v xml:space="preserve">Point2D_t  ktk_bwh_chest2 [] = {{500.,80.},{660.,80.},{660.,120.},{500.,120.},{.,.},{.,.},{.,.}};</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1">
@@ -24513,7 +24516,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I51" s="42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J51" s="43"/>
       <c r="K51" s="38"/>
@@ -24535,13 +24538,13 @@
         <v>125</v>
       </c>
       <c r="R51" s="61">
-        <v>25.5</v>
+        <v>30</v>
       </c>
       <c r="S51" s="49">
         <v>165</v>
       </c>
       <c r="T51" s="61">
-        <v>25.5</v>
+        <v>30</v>
       </c>
       <c r="U51" s="50">
         <v>165</v>
@@ -24569,7 +24572,7 @@
       </c>
       <c r="AF51" s="53">
         <f t="shared" si="49"/>
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="AG51" s="54">
         <f t="shared" si="49"/>
@@ -24577,7 +24580,7 @@
       </c>
       <c r="AH51" s="55">
         <f t="shared" si="49"/>
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="AI51" s="52">
         <f t="shared" si="49"/>
@@ -24621,7 +24624,7 @@
       </c>
       <c r="AS51" s="57" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">Point2D_t  ktk_atas_chest2 [] = {{500.,102.},{660.,102.},{660.,140.},{500.,140.},{.,.},{.,.},{.,.}};</v>
+        <v xml:space="preserve">Point2D_t  ktk_atas_chest2 [] = {{500.,120.},{660.,120.},{660.,140.},{500.,140.},{.,.},{.,.},{.,.}};</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1">
@@ -24759,7 +24762,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I53" s="42" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="J53" s="43"/>
       <c r="K53" s="38"/>
@@ -24865,7 +24868,7 @@
       </c>
       <c r="AS53" s="57" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">Point2D_t  putih_tulang [] = {{570.,102.},{586.,102.},{586.,140.},{570.,140.},{.,.},{.,.},{.,.}};</v>
+        <v xml:space="preserve">Point2D_t  ktk_kunci_chest2 [] = {{570.,102.},{586.,102.},{586.,140.},{570.,140.},{.,.},{.,.},{.,.}};</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1">
@@ -24886,7 +24889,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I54" s="42" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="J54" s="43"/>
       <c r="K54" s="38">
@@ -24982,7 +24985,7 @@
       </c>
       <c r="AS54" s="57" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">Color_t w_ktk_kunci_chest2 = {0.9,0.9,0.8};</v>
+        <v xml:space="preserve">Color_t putih_tulang = {0.9,0.9,0.8};</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1">
@@ -25003,7 +25006,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I55" s="42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J55" s="43">
         <v>4</v>
@@ -25042,7 +25045,7 @@
         <v>100</v>
       </c>
       <c r="W55" s="49">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="X55" s="43">
         <v>100</v>
@@ -25079,7 +25082,7 @@
       </c>
       <c r="AK55" s="54">
         <f t="shared" si="49"/>
-        <v>680</v>
+        <v>660</v>
       </c>
       <c r="AL55" s="55">
         <f t="shared" si="49"/>
@@ -25111,7 +25114,7 @@
       </c>
       <c r="AS55" s="57" t="str">
         <f t="shared" si="45"/>
-        <v xml:space="preserve">Point2D_t  ktk_jendela [4] = {{660.,280.},{780.,280.},{780.,400.},{680.,400.},{.,.},{.,.},{.,.}};</v>
+        <v xml:space="preserve">Point2D_t  ktk_jendela [4] = {{660.,280.},{780.,280.},{780.,400.},{660.,400.},{.,.},{.,.},{.,.}};</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1">
@@ -25132,7 +25135,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I56" s="42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J56" s="43"/>
       <c r="K56" s="38">
@@ -25249,7 +25252,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I57" s="42" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J57" s="43">
         <v>2</v>
@@ -25370,7 +25373,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I58" s="42" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J58" s="43">
         <v>2</v>
@@ -25491,7 +25494,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I59" s="42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J59" s="43">
         <v>2</v>
@@ -25612,7 +25615,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I60" s="42" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J60" s="43">
         <v>2</v>
@@ -25733,7 +25736,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I61" s="42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J61" s="43">
         <v>4</v>
@@ -25862,7 +25865,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I62" s="42" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J62" s="43"/>
       <c r="K62" s="38">
@@ -25979,7 +25982,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I63" s="42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J63" s="43">
         <v>4</v>
@@ -26108,7 +26111,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I64" s="42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J64" s="43"/>
       <c r="K64" s="38">
@@ -26225,7 +26228,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J65" s="43">
         <v>4</v>
@@ -26354,7 +26357,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I66" s="42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J66" s="43"/>
       <c r="K66" s="38">
@@ -26471,7 +26474,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I67" s="42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J67" s="43">
         <v>4</v>
@@ -26717,7 +26720,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I69" s="42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J69" s="43">
         <v>4</v>
@@ -26963,7 +26966,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I71" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J71" s="43"/>
       <c r="K71" s="38"/>
@@ -27207,7 +27210,7 @@
         <v>Point2D_t</v>
       </c>
       <c r="I73" s="42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J73" s="43"/>
       <c r="K73" s="38"/>
@@ -30783,7 +30786,7 @@
     <mergeCell ref="AO2:AP2"/>
     <mergeCell ref="AQ2:AR2"/>
   </mergeCells>
-  <dataValidations count="48" disablePrompts="0">
+  <dataValidations count="49" disablePrompts="0">
     <dataValidation sqref="N4:P105 I4:I12 I20 I22 I24:I25 I29 I31 I33 I35 I37 I39 I43 I47 I55 I61 I63 I67 I75:I105" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I14 I16 I18" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I27" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
@@ -30809,11 +30812,10 @@
     <dataValidation sqref="W51" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>#REF!=2</formula1>
     </dataValidation>
-    <dataValidation sqref="I49 I53" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
+    <dataValidation sqref="I49" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I50" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I51" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I52" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
-    <dataValidation sqref="I54" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I56" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I57" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I58" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
@@ -30840,6 +30842,8 @@
     <dataValidation sqref="I66" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I74" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
     <dataValidation sqref="I72" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
+    <dataValidation sqref="I53" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
+    <dataValidation sqref="I54" type="none" allowBlank="1" error="harus bilangan bulat antara 0 - 7" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1"/>
   </dataValidations>
   <printOptions headings="0" gridLines="0" horizontalCentered="1"/>
   <pageMargins left="0.19685039370078738" right="0.19685039370078738" top="0.39370078740157477" bottom="0.39370078740157477" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -30850,7 +30854,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{00AF006B-00D0-499F-99B5-006000D700F6}">
+          <x14:cfRule type="expression" priority="3" id="{000F0022-00E4-4B01-987D-00E700D7008B}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -30867,7 +30871,7 @@
           <xm:sqref>J4:J29 J31:J105 J31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{00DF00D5-0067-45FA-B585-0019000E000B}">
+          <x14:cfRule type="expression" priority="2" id="{006800BB-00AC-4CE8-BEB3-004E00660023}">
             <xm:f>$F4=2</xm:f>
             <x14:dxf>
               <font>
@@ -30884,7 +30888,7 @@
           <xm:sqref>K4:M105</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00380029-00E0-434F-938D-003B006300F4}">
+          <x14:cfRule type="expression" priority="1" id="{00E100E2-0082-456F-A4A6-007A00960090}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -30901,7 +30905,7 @@
           <xm:sqref>Q4:AD50 Y51:AD51 Q52:AD105</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{004900CE-003C-4C53-AEE0-008900BF00A1}">
+          <x14:cfRule type="expression" priority="1" id="{00FE009B-0075-4672-A027-006E00700086}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -30918,7 +30922,7 @@
           <xm:sqref>Q31:X31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00090061-0083-49FE-8F16-0018002E0013}">
+          <x14:cfRule type="expression" priority="1" id="{008A005D-004E-4F67-AACF-002C0082004C}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -30935,7 +30939,7 @@
           <xm:sqref>Q33:T33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00D6006A-0029-41E1-8E2F-0054007A0091}">
+          <x14:cfRule type="expression" priority="1" id="{00E70004-0012-4F57-A9B1-005700AB00B4}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -30952,7 +30956,7 @@
           <xm:sqref>U33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00260014-00E0-4685-B6EE-00B600A5008D}">
+          <x14:cfRule type="expression" priority="1" id="{008700F9-00D6-4501-A489-00F4007F00A9}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -30969,7 +30973,7 @@
           <xm:sqref>U33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00ED003C-0046-4BDA-89DF-0078009D009F}">
+          <x14:cfRule type="expression" priority="1" id="{002900B7-009B-4CDD-9DC7-000000670047}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -30986,7 +30990,7 @@
           <xm:sqref>Q41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{0068007D-0001-4ED7-8795-00A000540075}">
+          <x14:cfRule type="expression" priority="1" id="{00E7000F-00D4-4E32-879B-007700E4001E}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31003,7 +31007,7 @@
           <xm:sqref>S47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00880033-005D-42FB-B107-00F300D1007C}">
+          <x14:cfRule type="expression" priority="1" id="{002100BD-0088-4B78-B532-00830066007F}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31020,7 +31024,7 @@
           <xm:sqref>T47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{006900AD-0078-4ACA-8B44-006400EA0002}">
+          <x14:cfRule type="expression" priority="1" id="{00CE0090-0033-4A87-8D83-003A00B10007}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31037,7 +31041,7 @@
           <xm:sqref>U47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00E000DD-0098-4A6B-8E98-005C00250015}">
+          <x14:cfRule type="expression" priority="1" id="{004900A1-003F-492B-A7CD-00880090009B}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31054,7 +31058,7 @@
           <xm:sqref>U47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00FA002B-00D1-457E-9DA2-0054007D00EC}">
+          <x14:cfRule type="expression" priority="1" id="{006B003D-00DD-42EC-9C19-00CE00180023}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31071,7 +31075,7 @@
           <xm:sqref>W47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{007D0025-008B-497B-9B86-0058001E00A2}">
+          <x14:cfRule type="expression" priority="1" id="{004F00DD-00FE-4F48-BD1E-004100C00043}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31088,7 +31092,7 @@
           <xm:sqref>Q51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{001700A9-00B1-4401-87B4-000400890075}">
+          <x14:cfRule type="expression" priority="1" id="{00E60005-00E8-494B-BBEB-0058001700AF}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31105,7 +31109,7 @@
           <xm:sqref>S51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00890022-00E3-499D-8E30-0006000500D6}">
+          <x14:cfRule type="expression" priority="1" id="{00F000ED-00FF-4FCD-9981-005E008D0078}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31122,7 +31126,7 @@
           <xm:sqref>U51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00E900D9-0077-4747-A531-004C00760060}">
+          <x14:cfRule type="expression" priority="1" id="{00DC0070-0083-4699-8815-004600BB0018}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31139,7 +31143,7 @@
           <xm:sqref>W51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{0032008D-00AC-4ABD-9EA9-008700310095}">
+          <x14:cfRule type="expression" priority="1" id="{005F00DC-0076-41B0-B1A0-009800B10044}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31156,7 +31160,7 @@
           <xm:sqref>Q59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{0018004E-001B-4242-ADAE-007200910036}">
+          <x14:cfRule type="expression" priority="1" id="{009400BE-009C-401C-A5C1-00960034008D}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31173,7 +31177,7 @@
           <xm:sqref>S59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00990046-007B-4638-8AD4-005900550020}">
+          <x14:cfRule type="expression" priority="1" id="{003400E7-0024-491C-824F-0037001C0029}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31190,7 +31194,7 @@
           <xm:sqref>Q60:T60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{009E0022-0051-4B09-8DF4-0078009200F1}">
+          <x14:cfRule type="expression" priority="1" id="{00F50055-00A8-43B1-8E1A-0038002D00E0}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31207,7 +31211,7 @@
           <xm:sqref>W61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{008B0072-003B-4955-9D75-00AE00A90083}">
+          <x14:cfRule type="expression" priority="1" id="{00F10069-005D-4264-A72B-008100EE005A}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31224,7 +31228,7 @@
           <xm:sqref>X61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{001F0026-0011-4AFF-9CCC-00C300E400CC}">
+          <x14:cfRule type="expression" priority="1" id="{00C50041-0088-4A9C-937D-00CA00000091}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31241,7 +31245,7 @@
           <xm:sqref>V63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00EC0038-0022-42FB-985D-00DC007F0066}">
+          <x14:cfRule type="expression" priority="1" id="{007D00F5-00A3-449D-9BD2-00BC007900A5}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31258,7 +31262,7 @@
           <xm:sqref>X63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{0084005B-0047-4A01-9186-002500B000B4}">
+          <x14:cfRule type="expression" priority="1" id="{00300076-004C-47D6-B4F0-00F6002D00D0}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31275,7 +31279,7 @@
           <xm:sqref>X63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{001000D1-0037-4944-96B0-00C4000900F0}">
+          <x14:cfRule type="expression" priority="1" id="{00E7008F-00A3-4C55-A10F-003A00F8003A}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31292,7 +31296,7 @@
           <xm:sqref>X65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{000C003A-0044-48A5-B3A4-001E0094001B}">
+          <x14:cfRule type="expression" priority="1" id="{00870005-00D6-4CE2-8D66-0094005900A3}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31309,7 +31313,7 @@
           <xm:sqref>U67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00EE00AB-00E3-4539-96BD-00AB001700C4}">
+          <x14:cfRule type="expression" priority="1" id="{0034006A-003D-4664-8755-004800C1004F}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31326,7 +31330,7 @@
           <xm:sqref>U69:X69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00070019-0007-4C17-A4EE-00AB00D00093}">
+          <x14:cfRule type="expression" priority="1" id="{00E60070-002C-42AC-BAB9-00B60060006A}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31343,7 +31347,7 @@
           <xm:sqref>U71:X71</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00300065-001E-4E14-B4EF-004D00DD0010}">
+          <x14:cfRule type="expression" priority="1" id="{00F10061-0014-454E-8E01-008400AA0024}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31360,7 +31364,7 @@
           <xm:sqref>U73:X73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{008C0063-0085-4DC8-BD82-004B008400B2}">
+          <x14:cfRule type="expression" priority="1" id="{001A00D6-0036-41CB-8C51-003100F5006D}">
             <xm:f>$F4=1</xm:f>
             <x14:dxf>
               <font>
@@ -31380,25 +31384,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="30" disablePrompts="0">
-        <x14:dataValidation xr:uid="{008400C4-00F7-4FF1-830C-004B000E009C}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C6008F-0071-485B-A433-0007001E00F7}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>Q4:AD30 Y31:AD31 Q32:AD32 V33:AD33 Q34:AD40 R41:AD41 Q42:AD46 Q47:R47 V47 X47:AD47 Q48:AD50 Y51:AD51 Q52:AD58 R59 T59:AD59 U60:AD60 Q61:V61 Y61:AD61 Q62:AD62 Q63:U63 W63 Y63:AD63 Q64:AD64 Q65:W65 Y65:AD65 Q66:AD66 Q67:T67 V67:AD67 Q68:AD68 Q69:T69 Y69:AD69 Q70:AD70 Q71:T71 Y71:AD71 Q72:AD72 Q73:T73 Y73:AD73 Q74:AD105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008700E6-0032-4876-933A-0019006F00C7}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Isi dengan angka 0 - 255" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00960064-0077-4E72-A4CB-0006004500D1}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Isi dengan angka 0 - 255" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>AND($F4=1,K4&gt;=0,K4&lt;256)</xm:f>
           </x14:formula1>
           <xm:sqref>K4:M8 K10:M10 K12:M20 K22:M105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00030054-0041-4051-9D70-00DC0033000F}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Diisi banyaknya titik" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006A0061-0071-46FD-AC64-001000E90021}" type="custom" allowBlank="1" error="Angka tidak valid atau tidak boleh diisi" errorStyle="stop" errorTitle="ERROR" imeMode="noControl" operator="between" prompt="Diisi banyaknya titik" promptTitle="INFORMASI" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>AND(F4=2,J4&gt;0)</xm:f>
           </x14:formula1>
           <xm:sqref>J4:J29 J31 J32:J105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C1001A-00BE-4224-846C-005B009F00C5}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BF004D-0090-4EC8-AFDE-00BA00920067}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>1</xm:f>
           </x14:formula1>
@@ -31407,25 +31411,25 @@
           </x14:formula2>
           <xm:sqref>F4:F13 F20:F60 F63:F105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00240043-005B-475D-8E24-0097006600CD}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 1024" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009600D0-00A9-4BC5-8F7C-001A005400AF}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 1024" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>1024</xm:f>
           </x14:formula1>
           <xm:sqref>A4 C4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009D00C8-00EA-4E8E-8BCA-0003005C00CA}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 768" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006F00F7-0079-4F4E-86CB-001400D700EF}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= 768" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>768</xm:f>
           </x14:formula1>
           <xm:sqref>B4 D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AB0072-0015-4DE5-953F-00C100A4001D}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= LEBAR DESAIN" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E000C9-0040-4979-8585-00DF00080062}" type="whole" allowBlank="1" error="harus bilangan bulat &lt;= LEBAR DESAIN" errorStyle="stop" imeMode="noControl" operator="lessThanOrEqual" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>AF4:AR105</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0059009A-0053-428C-9E78-003900CD00B4}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C30059-0060-4614-8BC0-0013008300D2}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>1</xm:f>
           </x14:formula1>
@@ -31434,85 +31438,85 @@
           </x14:formula2>
           <xm:sqref>F14:F19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0056003B-005A-4B8C-8C93-0017003100B9}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000B000F-009E-421C-9EBB-00CD007300B4}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F5=2</xm:f>
           </x14:formula1>
           <xm:sqref>Q31:X31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004600E2-005F-4A28-A641-0097003E00B6}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FF0032-0064-429D-A192-006C00240075}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F8=2</xm:f>
           </x14:formula1>
           <xm:sqref>Q33:T33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006D0094-0027-43B9-91DF-00B500A30003}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002300C6-0027-4C51-A572-005E0011006C}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F8=2</xm:f>
           </x14:formula1>
           <xm:sqref>U33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DA00DA-00E0-4020-B589-004600CD00F5}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00ED0082-0016-4539-B125-00BD00D900AB}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F6=2</xm:f>
           </x14:formula1>
           <xm:sqref>Q41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000200F4-002B-4D4C-A482-00F000F10011}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006200B1-0075-45ED-929F-0066004F0089}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>S47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EE00D8-0029-47EB-AA7A-0047008B006A}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EE0035-0058-4C82-B2AD-0025001E0099}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>T47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AA00F3-006B-4DB5-8994-00D7008D00CC}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006600DE-0099-42BB-A274-00D300930069}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>U47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002B0033-0005-441A-8003-002B00390038}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003C0098-00A7-46B2-813F-0025009C0072}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>W47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B90045-00BD-4A4F-A79A-00C9002300F6}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000D0046-0093-4D74-83F4-00E200FE00F6}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F6=2</xm:f>
           </x14:formula1>
           <xm:sqref>Q59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00810022-0024-44B5-BCBA-004B008C0048}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002D0021-0079-48C4-B59F-0044006C00B1}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F6=2</xm:f>
           </x14:formula1>
           <xm:sqref>S59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009D0010-00FA-4465-9179-000700F900B1}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0001002E-00C7-438E-8626-00E800F5000D}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F6=2</xm:f>
           </x14:formula1>
           <xm:sqref>Q60:T60</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00370079-0029-4940-BBA6-00F6003B0033}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F00051-0045-48FA-863B-00AC00530063}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>W61</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00470055-00BE-45FF-A72B-00790042004D}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007800C5-001B-40C7-AF7A-00D400330043}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>X61</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00760081-009D-4CC4-8891-007B00A0004A}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008F0078-00CD-4D82-868A-00AC00090087}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>1</xm:f>
           </x14:formula1>
@@ -31521,7 +31525,7 @@
           </x14:formula2>
           <xm:sqref>F61</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B50099-00ED-4182-AE0A-00DC00880096}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008B0052-0085-4B28-9825-0057006100C2}" type="whole" allowBlank="1" error="harus angka 1 atau 2" errorStyle="stop" errorTitle="Salah" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>1</xm:f>
           </x14:formula1>
@@ -31530,43 +31534,43 @@
           </x14:formula2>
           <xm:sqref>F62</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000600A0-007C-49B9-96DF-0003008F0028}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008700C3-00F2-4B43-AAAA-00A000FE00D8}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F6=2</xm:f>
           </x14:formula1>
           <xm:sqref>V63</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00220004-00F7-43D8-9F6C-00A2001900BE}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00390065-0003-44B2-AE12-003E00970025}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F6=2</xm:f>
           </x14:formula1>
           <xm:sqref>X63</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B300D2-00A3-4D1C-9023-0022007F0097}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A1001E-00FD-49DE-AA99-00840011000C}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>X65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C40062-0047-489B-ACF4-00AE00AE002B}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D40011-0044-47FB-87A9-00F20076005E}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>U67</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009F0096-00CD-40E1-8D11-002D006500D7}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C9000D-0069-45A3-8B0C-00A600B10042}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>U69:X69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C600E1-0061-4B2F-AB66-005C003800E6}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005B00ED-001A-444F-AA64-00B5004B0001}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F4=2</xm:f>
           </x14:formula1>
           <xm:sqref>U71:X71</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D100B0-00F4-4BA6-8030-0022000300E0}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CC00AB-0009-4B6E-AEBF-00EA0071002B}" type="custom" allowBlank="1" error="Tidak boleh diisi" errorStyle="stop" errorTitle="Error" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$F6=2</xm:f>
           </x14:formula1>

</xml_diff>